<commit_message>
add Kinect To Amin
Kinect 130Dt le 2 mars 2020
</commit_message>
<xml_diff>
--- a/Team Mangement/FichierAchat.xlsx
+++ b/Team Mangement/FichierAchat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\USER_ismail\RobotCartesién\MechanicalDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\USER_ismail\RobotCartesién\Team Mangement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t xml:space="preserve">Courroie </t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t xml:space="preserve">total </t>
+  </si>
+  <si>
+    <t>Kinect</t>
   </si>
 </sst>
 </file>
@@ -476,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,6 +716,12 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18">
+        <v>130</v>
+      </c>
       <c r="H18">
         <v>25</v>
       </c>
@@ -728,6 +737,11 @@
       <c r="L18">
         <f>SUM(H18:K18)</f>
         <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>